<commit_message>
Cleansingf the database report folder
</commit_message>
<xml_diff>
--- a/ISAD/03 - Work plan.xlsx
+++ b/ISAD/03 - Work plan.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kmitlthailand.sharepoint.com/sites/ProjectFountain926/Shared Documents/panda-report/ISAD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kumamon/KMITL/Project Panda - Documents/panda-report/ISAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_046D7EC2F8FF96B187FB09BC5018844F176281C0" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{21F48AA5-DA4F-47F9-B90B-117D5C141BD1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE63C7F-E2DF-5540-B68F-E486C1A36DB6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="17565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="440" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Table" sheetId="1" r:id="rId1"/>
     <sheet name="Gannt Chart" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Task Table'!$A:$I</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Task Table'!$A$1:$H$46,'Task Table'!$I:$I</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Task Table'!$2:$4</definedName>
   </definedNames>
   <calcPr calcId="179017" concurrentCalc="0"/>
@@ -372,6 +372,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -385,9 +388,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1983,31 +1983,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF3D85C6"/>
-    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
+      <selection pane="bottomLeft" activeCell="I1" activeCellId="1" sqref="A1:H46 I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="27" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.7109375" style="29" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="8"/>
-    <col min="11" max="16384" width="14.42578125" style="7"/>
+    <col min="1" max="1" width="4.83203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.6640625" style="29" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="4.83203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="8"/>
+    <col min="11" max="16384" width="14.5" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2017,51 +2016,51 @@
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="32"/>
-    </row>
-    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="33"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="32"/>
-    </row>
-    <row r="5" spans="1:8" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="33"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="11">
         <v>1</v>
@@ -2084,7 +2083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="16">
         <v>1.1000000000000001</v>
@@ -2109,7 +2108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="16">
         <v>1.2</v>
@@ -2134,7 +2133,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="16">
         <v>1.3</v>
@@ -2159,7 +2158,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20"/>
@@ -2169,7 +2168,7 @@
       <c r="G9" s="21"/>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="22">
         <v>2</v>
@@ -2192,7 +2191,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="16">
         <v>2.1</v>
@@ -2217,7 +2216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="16">
         <v>2.2000000000000002</v>
@@ -2242,7 +2241,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="16">
         <v>2.2999999999999998</v>
@@ -2267,7 +2266,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="16">
         <v>2.4</v>
@@ -2292,7 +2291,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="19"/>
       <c r="C15" s="20"/>
@@ -2302,7 +2301,7 @@
       <c r="G15" s="21"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="19">
         <v>3</v>
@@ -2325,7 +2324,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="16">
         <v>3.1</v>
@@ -2350,7 +2349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="16">
         <v>3.2</v>
@@ -2375,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="16">
         <v>3.3</v>
@@ -2400,7 +2399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="16">
         <v>3.4</v>
@@ -2425,7 +2424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="16">
         <v>3.5</v>
@@ -2450,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="19"/>
       <c r="C22" s="20"/>
@@ -2460,7 +2459,7 @@
       <c r="G22" s="21"/>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="19">
         <v>4</v>
@@ -2483,7 +2482,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="16">
         <v>4.0999999999999996</v>
@@ -2508,7 +2507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="16">
         <v>4.2</v>
@@ -2533,7 +2532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="16">
         <v>4.3</v>
@@ -2558,7 +2557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="16">
         <v>4.4000000000000004</v>
@@ -2586,7 +2585,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="19"/>
       <c r="C28" s="20"/>
@@ -2596,7 +2595,7 @@
       <c r="G28" s="21"/>
       <c r="H28" s="24"/>
     </row>
-    <row r="29" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="19">
         <v>5</v>
@@ -2619,7 +2618,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="16">
         <v>5.0999999999999996</v>
@@ -2644,7 +2643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="16">
         <v>5.2</v>
@@ -2669,7 +2668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="16">
         <v>5.3</v>
@@ -2694,7 +2693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="16">
         <v>5.4</v>
@@ -2719,7 +2718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="19"/>
       <c r="C34" s="20"/>
@@ -2729,7 +2728,7 @@
       <c r="G34" s="25"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="19">
         <v>6</v>
@@ -2752,7 +2751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="16">
         <v>6.1</v>
@@ -2777,7 +2776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="16">
         <v>6.2</v>
@@ -2802,7 +2801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="16">
         <v>6.3</v>
@@ -2827,60 +2826,60 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="30">
         <v>1</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="C41" s="31" t="s">
         <v>46</v>
       </c>
       <c r="D41" s="28">
         <v>59070009</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="30">
         <v>2</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="31" t="s">
         <v>47</v>
       </c>
       <c r="D42" s="28">
         <v>59070022</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="30">
         <v>3</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="C43" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D43" s="28">
         <v>59070043</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="30">
         <v>4</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="31" t="s">
         <v>49</v>
       </c>
       <c r="D44" s="28">
         <v>59070087</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="30">
         <v>5</v>
       </c>
-      <c r="C45" s="37" t="s">
+      <c r="C45" s="31" t="s">
         <v>50</v>
       </c>
       <c r="D45" s="28">
@@ -2898,7 +2897,7 @@
     <mergeCell ref="D2:D4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="75" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2909,6 +2908,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F05C1EF0044CF249A09568BFC7A27DEF" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a308155717e7f8eadebf0d848e17ba4f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="360d23a6-f195-4c5c-b5bb-19aa4319b9ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1d6afd8dd879a1d7a61ed4bc2f66470" ns2:_="">
     <xsd:import namespace="360d23a6-f195-4c5c-b5bb-19aa4319b9ef"/>
@@ -3060,15 +3068,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84BAB9AF-D7E3-4935-902D-F19D2D3AE227}">
   <ds:schemaRefs>
@@ -3086,6 +3085,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FB229F0-8222-4E0E-98F5-97B5EFBD90CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2627D2E6-4B24-4613-8E49-3AC75E278B25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3101,12 +3108,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FB229F0-8222-4E0E-98F5-97B5EFBD90CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>